<commit_message>
agregar contador de documentos a incidencias
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,7 +517,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01233421</t>
+          <t>01374859</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -537,35 +537,44 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>V530</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J2" t="n">
-        <v>8013913</v>
+          <t>M700z</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>8013913</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Biobío</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Los Angeles</t>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>02988776</t>
+          <t>02993344</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>VILLA GENESIS</t>
+          <t>BALDOMERO LILLO</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -580,14 +589,18 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>V510z</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>17006716</v>
+          <t>71z</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>8013913</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -598,22 +611,22 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Coronel</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>OFICINA</t>
+          <t>CLASICO</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>01374859</t>
+          <t>01773356</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BALDOMERO LILLO</t>
+          <t>ABKELAY KIMUN</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -628,83 +641,91 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>M700z</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>8013913</v>
+          <t>E73z</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>8013913</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Concepcion</t>
+          <t>V530</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01233421</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
           <t>Coronel</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>02993344</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>71z</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>8013913</v>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>8013913</t>
+        </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Arauco</t>
+          <t>V510z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tirúa</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>01773356</t>
+          <t>02988776</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>ABKELAY KIMUN</t>
+          <t>VILLA GENESIS</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -719,14 +740,117 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>E73z</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>8013913</v>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>17006716</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>V530</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01233421</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>8013913</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>V510z</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>02988776</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>VILLA GENESIS</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>17006716</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -1238,7 +1362,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1313,27 +1437,32 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Arauco</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tirúa</t>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>123</t>
+          <t>001</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>ABKELAY KIMUN</t>
+          <t>BALDOMERO LILLO</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Teclado</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -1346,11 +1475,15 @@
           <t>S3 SERIES</t>
         </is>
       </c>
-      <c r="I2" t="n">
-        <v>123</v>
-      </c>
-      <c r="J2" t="n">
-        <v>123</v>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>0001</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -1361,22 +1494,22 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Coronel</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OFICINA</t>
+          <t>CLASICO</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00137</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>BALDOMERO LILLO</t>
+          <t>ABKELAY KIMUN</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -1386,62 +1519,169 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Lenovo</t>
+          <t>ACER</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>V510z</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>137</v>
-      </c>
-      <c r="J3" t="n">
-        <v>137</v>
+          <t>S3 SERIES</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>00137</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Teclado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>V510z</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Biobío</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>Los Angeles</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>2A</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>VILLA GENESIS</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>CPU</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>HP</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>340</t>
         </is>
       </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="n">
-        <v>2</v>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Santa Juana</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>356734</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Nueva-Unidad</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>S3 SERIES</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2346</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0839433</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cambiar el modelo de tipo_equipo combinado con marca y modelo
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="AIO" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Impresoras" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Bam" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Proyectoes" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Telefonos" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Disco Duro" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Tablets" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Otros" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="sheet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Notebooks" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Impresoras" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Bam" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Proyectoes" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Telefonos" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Disco Duro" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Tablets" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Otros" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="sheet" sheetId="10" state="visible" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -427,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +446,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -475,195 +478,229 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Concepcion</t>
+          <t>V530</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>01233421</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>8015892</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
           <t>Coronel</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>01374859</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>M700z</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="K2" t="inlineStr">
         <is>
           <t>8013913</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>Sonda</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>V510z</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CLASICO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>02988776</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>ABKELAY KIMUN</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>8203001</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>Concepcion</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>02993344</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>71z</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>8013913</t>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>17006716</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>Sonda</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Concepcion</t>
+          <t>M700z</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Concepcion</t>
+          <t>3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CLASICO</t>
+          <t>OFICINA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>01773356</t>
+          <t>01374859</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ABKELAY KIMUN</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>8015892</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>AIO</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Lenovo</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>E73z</t>
-        </is>
-      </c>
       <c r="I4" t="inlineStr">
         <is>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>8013913</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Sonda</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>V530</t>
+          <t>71z</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -673,7 +710,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>01233421</t>
+          <t>02993344</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -681,179 +718,119 @@
           <t>BALDOMERO LILLO</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>8015892</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>AIO</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Lenovo</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Coronel</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>8013913</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>Sonda</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>V510z</t>
+          <t>E73z</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CLASICO</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>02988776</t>
+          <t>01773356</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>VILLA GENESIS</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
+          <t>ABKELAY KIMUN</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>8203001</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>AIO</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Lenovo</t>
         </is>
       </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
       <c r="I6" t="inlineStr">
         <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>17006716</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>V530</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>01233421</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
+      <c r="K6" t="inlineStr">
         <is>
           <t>8013913</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>V510z</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>02988776</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>VILLA GENESIS</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>17006716</t>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>Sonda</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -864,7 +841,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -882,6 +859,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -912,27 +891,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -947,7 +936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -965,6 +954,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -995,27 +986,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1048,6 +1049,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1078,27 +1081,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1113,7 +1126,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1131,6 +1144,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1161,27 +1176,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1214,6 +1239,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1244,27 +1271,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1279,7 +1316,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1297,6 +1334,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1327,27 +1366,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1380,6 +1429,8 @@
     <col width="20" customWidth="1" min="8" max="8"/>
     <col width="20" customWidth="1" min="9" max="9"/>
     <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1410,277 +1461,37 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>CodigoUnidad</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>Tipo de Bien</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Marca</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Modelo</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>N° Serie</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Codigo Inventario</t>
         </is>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>001</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>ACER</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>S3 SERIES</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>0001</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>ABKELAY KIMUN</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Teclado</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ACER</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>S3 SERIES</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>00137</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Teclado</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>V510z</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>137</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>137</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Biobío</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>VILLA GENESIS</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>CPU</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>HP</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>340</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Santa Juana</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>356734</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Nueva-Unidad</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>ACER</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>S3 SERIES</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2346</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>0839433</t>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
         </is>
       </c>
     </row>
@@ -1695,14 +1506,298 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Provincia</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Comuna</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Modalidad</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Codigo Proveedor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Tipo de Bien</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Marca</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Modelo</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>N° Serie</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Codigo Inventario</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Nombre Proveedor</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Biobío</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2A</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>VILLA GENESIS</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CPU</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>340</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Sonda</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>S3 SERIES</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>VILLA GENESIS</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Teclado</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Los Angeles</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Sonda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>V510z</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>00137</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Teclado</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>137</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sonda</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>S3 SERIES</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>356734</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Nueva-Unidad</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ACER</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Santa Juana</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2346</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0839433</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Sonda</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
resolver errores de tipo_equipo y resolver problema de tablas en sql con mayusculas no funcionando en linux
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,12 +515,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>V530</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Coronel</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>01233421</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -553,17 +553,17 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Coronel</t>
+          <t>V2414</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>123</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>8013913</t>
+          <t>123</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -575,31 +575,31 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>V510z</t>
+          <t>Concepcion</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Coronel</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CLASICO</t>
+          <t>OFICINA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>02988776</t>
+          <t>123</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ABKELAY KIMUN</t>
+          <t>BALDOMERO LILLO</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>8203001</v>
+        <v>8015892</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -613,200 +613,20 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Concepcion</t>
+          <t>V2414</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>123</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>17006716</t>
+          <t>123</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>M700z</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>01374859</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>8015892</v>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>8013913</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>71z</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>02993344</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>8015892</v>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>8013913</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>E73z</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>CLASICO</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>01773356</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>ABKELAY KIMUN</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>8203001</v>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>AIO</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Concepcion</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>8013913</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
         <is>
           <t>Sonda</t>
         </is>
@@ -1506,7 +1326,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1584,219 +1404,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Biobío</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>2A</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>VILLA GENESIS</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>CPU</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>HP</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>340</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>S3 SERIES</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>VILLA GENESIS</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Teclado</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>ACER</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Los Angeles</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>123</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>V510z</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>OFICINA</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>00137</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>BALDOMERO LILLO</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Teclado</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Lenovo</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Coronel</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>137</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>137</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>S3 SERIES</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>356734</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Nueva-Unidad</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Mouse</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>ACER</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Santa Juana</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2346</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>0839433</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Sonda</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
arreglar error con exportar datos
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,35 +515,211 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>1235134</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>u_de_excel</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Telefono</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>123Z</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>p2000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>3245234512</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>forzado</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CLASICO</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>758</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>u_de_excel</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>123X</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>123Z</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>123M</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>584</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>forzado</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CLASICO</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>123</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>ABKELAY KIMUN</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>test</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>TEST_MODELO</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>todo en uno1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>123</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Sonda</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Concepcion</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Coronel</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>OFICINA</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>34634</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>BALDOMERO LILLO</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>AIO</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>todo en uno1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>43625234</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>142365</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Sonda</t>
         </is>

</xml_diff>